<commit_message>
Added utils and made the changes to incorporate TestNG
</commit_message>
<xml_diff>
--- a/POC/TD.xlsx
+++ b/POC/TD.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nisum/Desktop/Testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nisum/git/Automationpractice/POC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E985D3CE-3FC8-3842-9228-6983DB277EE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3141CA6A-3409-7349-B5B9-19A36E827860}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{C044B65A-D823-514A-BF4C-A552A954B30A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{C044B65A-D823-514A-BF4C-A552A954B30A}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Object" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Value</t>
   </si>
@@ -117,13 +117,67 @@
   </si>
   <si>
     <t>36104</t>
+  </si>
+  <si>
+    <t>login_btn</t>
+  </si>
+  <si>
+    <t>className:login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uname </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id:email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id:passwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submit_btn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id:SubmitLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logout </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> className:logout</t>
+  </si>
+  <si>
+    <t>id:email</t>
+  </si>
+  <si>
+    <t>id:passwd</t>
+  </si>
+  <si>
+    <t>id:SubmitLogin</t>
+  </si>
+  <si>
+    <t>className:logout</t>
+  </si>
+  <si>
+    <t>uname</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>submit_btn</t>
+  </si>
+  <si>
+    <t>logout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +212,13 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -202,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -216,6 +277,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -533,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F05EFD-0B05-7144-BC13-DA7991301286}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,118 +762,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510ABB7E-FA2F-C147-B6E8-9BD1D18540DE}">
-  <dimension ref="F1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -818,20 +911,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE469C9-3B3D-EA47-BB0F-7A2D9B86CF52}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J7" sqref="J7:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="str">
+        <f>CLEAN(TRIM(H7))</f>
+        <v>uname</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ref="J8:J10" si="0">CLEAN(TRIM(H8))</f>
+        <v>password</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>submit_btn</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>logout</v>
       </c>
     </row>
   </sheetData>

</xml_diff>